<commit_message>
4/04 optimizing variogram parameters for area1
new boundaries were used
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/optimal_nugget_range_value.xlsx
+++ b/_INTERPOLATION/optimal_nugget_range_value.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\python_map\New\Vistelius_1995_OCR\_INTERPOLATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ACE6A2-1C0C-4B7A-AAD5-24C8A9A8A4B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8EF193-D4C6-406A-AD17-F87D1F342487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B3A2F8EB-B1AE-45BB-BB45-54B64F4D81FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B3A2F8EB-B1AE-45BB-BB45-54B64F4D81FD}"/>
   </bookViews>
   <sheets>
     <sheet name="# control points" sheetId="7" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="24">
   <si>
     <t>range</t>
   </si>
@@ -102,6 +102,15 @@
   <si>
     <t>same</t>
   </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>new boundaries</t>
+  </si>
+  <si>
+    <t>.....</t>
+  </si>
 </sst>
 </file>
 
@@ -122,7 +131,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +174,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -193,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -203,6 +218,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -519,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A5B619B-5250-4BC6-8A52-0322DD650F59}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -639,18 +658,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B424C6FD-858B-4715-AB2E-8F192D327931}">
-  <dimension ref="A2:W26"/>
+  <dimension ref="A1:AL27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T25" activeCellId="6" sqref="Q19 S20 R21 S22 S23 S24 T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -712,8 +737,41 @@
       <c r="W2" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AB2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="AD2" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -782,8 +840,43 @@
         <f t="shared" si="1"/>
         <v>1.236</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AB3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="7">
+        <v>1.0517000000000001</v>
+      </c>
+      <c r="AD3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE3" s="4">
+        <v>1.0351999999999999</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>1.0343100000000001</v>
+      </c>
+      <c r="AG3" s="4">
+        <v>1.0345500000000001</v>
+      </c>
+      <c r="AH3">
+        <v>1.0388599999999999</v>
+      </c>
+      <c r="AI3">
+        <v>1.0471999999999999</v>
+      </c>
+      <c r="AJ3">
+        <v>1.0601700000000001</v>
+      </c>
+      <c r="AK3">
+        <v>1.0808500000000001</v>
+      </c>
+      <c r="AL3">
+        <v>1.12018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <f>B3+1</f>
         <v>2</v>
@@ -854,8 +947,46 @@
         <f t="shared" si="3"/>
         <v>0.78500000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Y4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z4" s="3"/>
+      <c r="AB4" s="2">
+        <f>AB3+1</f>
+        <v>2</v>
+      </c>
+      <c r="AC4" s="7">
+        <v>0.63160000000000005</v>
+      </c>
+      <c r="AD4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>0.61319999999999997</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>0.61240000000000006</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>0.61226999999999998</v>
+      </c>
+      <c r="AH4">
+        <v>0.61481200000000003</v>
+      </c>
+      <c r="AI4">
+        <v>0.62050000000000005</v>
+      </c>
+      <c r="AJ4">
+        <v>0.63029999999999997</v>
+      </c>
+      <c r="AK4">
+        <v>0.64649999999999996</v>
+      </c>
+      <c r="AL4">
+        <v>0.67700000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <f t="shared" ref="B5:B10" si="5">B4+1</f>
         <v>3</v>
@@ -926,8 +1057,42 @@
         <f t="shared" si="7"/>
         <v>0.58450000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AB5" s="2">
+        <f t="shared" ref="AB5:AB10" si="9">AB4+1</f>
+        <v>3</v>
+      </c>
+      <c r="AC5" s="7">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="AD5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE5">
+        <v>0.44340000000000002</v>
+      </c>
+      <c r="AF5">
+        <v>0.44112000000000001</v>
+      </c>
+      <c r="AG5">
+        <v>0.43790000000000001</v>
+      </c>
+      <c r="AH5">
+        <v>0.435172</v>
+      </c>
+      <c r="AI5" s="3">
+        <v>0.43409999999999999</v>
+      </c>
+      <c r="AJ5">
+        <v>0.43530000000000002</v>
+      </c>
+      <c r="AK5">
+        <v>0.43890000000000001</v>
+      </c>
+      <c r="AL5">
+        <v>0.44790000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -959,47 +1124,81 @@
         <v>4.8250000000000001E-2</v>
       </c>
       <c r="N6">
-        <f t="shared" ref="N6:W6" si="9">$K$6*N2</f>
+        <f t="shared" ref="N6:W6" si="10">$K$6*N2</f>
         <v>9.6500000000000002E-2</v>
       </c>
       <c r="O6">
+        <f t="shared" si="10"/>
+        <v>0.14474999999999999</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6" si="11">$K$6*P2</f>
+        <v>0.15922500000000001</v>
+      </c>
+      <c r="Q6" s="7">
+        <f t="shared" si="10"/>
+        <v>0.193</v>
+      </c>
+      <c r="R6" s="7">
+        <f t="shared" si="10"/>
+        <v>0.24124999999999999</v>
+      </c>
+      <c r="S6" s="3">
+        <f t="shared" si="10"/>
+        <v>0.28949999999999998</v>
+      </c>
+      <c r="T6" s="7">
+        <f t="shared" si="10"/>
+        <v>0.33774999999999999</v>
+      </c>
+      <c r="U6" s="7">
+        <f t="shared" si="10"/>
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="V6" s="7">
+        <f t="shared" si="10"/>
+        <v>0.43424999999999997</v>
+      </c>
+      <c r="W6" s="7">
+        <f t="shared" si="10"/>
+        <v>0.48249999999999998</v>
+      </c>
+      <c r="AB6" s="2">
         <f t="shared" si="9"/>
-        <v>0.14474999999999999</v>
-      </c>
-      <c r="P6">
-        <f t="shared" ref="P6" si="10">$K$6*P2</f>
-        <v>0.15922500000000001</v>
-      </c>
-      <c r="Q6" s="7">
-        <f t="shared" si="9"/>
-        <v>0.193</v>
-      </c>
-      <c r="R6" s="7">
-        <f t="shared" si="9"/>
-        <v>0.24124999999999999</v>
-      </c>
-      <c r="S6" s="3">
-        <f t="shared" si="9"/>
-        <v>0.28949999999999998</v>
-      </c>
-      <c r="T6" s="7">
-        <f t="shared" si="9"/>
-        <v>0.33774999999999999</v>
-      </c>
-      <c r="U6" s="7">
-        <f t="shared" si="9"/>
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="V6" s="7">
-        <f t="shared" si="9"/>
-        <v>0.43424999999999997</v>
-      </c>
-      <c r="W6" s="7">
-        <f t="shared" si="9"/>
-        <v>0.48249999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="AC6" s="7">
+        <v>0.47339999999999999</v>
+      </c>
+      <c r="AD6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE6">
+        <v>0.45989999999999998</v>
+      </c>
+      <c r="AF6">
+        <v>0.45856000000000002</v>
+      </c>
+      <c r="AG6">
+        <v>0.45660000000000001</v>
+      </c>
+      <c r="AH6">
+        <v>0.45506799999999997</v>
+      </c>
+      <c r="AI6" s="3">
+        <v>0.45450000000000002</v>
+      </c>
+      <c r="AJ6">
+        <v>0.45469999999999999</v>
+      </c>
+      <c r="AK6">
+        <v>0.45579999999999998</v>
+      </c>
+      <c r="AL6">
+        <v>0.45800000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <f t="shared" si="5"/>
         <v>5</v>
@@ -1031,47 +1230,81 @@
         <v>3.1219999999999998E-2</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="N7:W7" si="11">$K$7*N2</f>
+        <f t="shared" ref="N7:W7" si="12">$K$7*N2</f>
         <v>6.2439999999999996E-2</v>
       </c>
       <c r="O7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9.3659999999999993E-2</v>
       </c>
       <c r="P7">
-        <f t="shared" ref="P7" si="12">$K$7*P2</f>
+        <f t="shared" ref="P7" si="13">$K$7*P2</f>
         <v>0.10302599999999999</v>
       </c>
       <c r="Q7" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.12487999999999999</v>
       </c>
       <c r="R7" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.15609999999999999</v>
       </c>
       <c r="S7" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.18731999999999999</v>
       </c>
       <c r="T7" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.21853999999999998</v>
       </c>
       <c r="U7" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.24975999999999998</v>
       </c>
       <c r="V7" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.28098000000000001</v>
       </c>
       <c r="W7" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.31219999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AB7" s="2">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="AC7" s="7">
+        <v>0.31059999999999999</v>
+      </c>
+      <c r="AD7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE7">
+        <v>0.29770000000000002</v>
+      </c>
+      <c r="AF7">
+        <v>0.29703000000000002</v>
+      </c>
+      <c r="AG7">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="AH7" s="3">
+        <v>0.29538900000000001</v>
+      </c>
+      <c r="AI7">
+        <v>0.29565000000000002</v>
+      </c>
+      <c r="AJ7">
+        <v>0.29670000000000002</v>
+      </c>
+      <c r="AK7">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="AL7">
+        <v>0.3034</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -1103,47 +1336,81 @@
         <v>2.92E-2</v>
       </c>
       <c r="N8">
-        <f t="shared" ref="N8:W8" si="13">$K$8*N2</f>
+        <f t="shared" ref="N8:W8" si="14">$K$8*N2</f>
         <v>5.8400000000000001E-2</v>
       </c>
       <c r="O8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8.7599999999999997E-2</v>
       </c>
       <c r="P8">
-        <f t="shared" ref="P8" si="14">$K$8*P2</f>
+        <f t="shared" ref="P8" si="15">$K$8*P2</f>
         <v>9.6360000000000001E-2</v>
       </c>
       <c r="Q8" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.1168</v>
       </c>
       <c r="R8" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.14599999999999999</v>
       </c>
       <c r="S8" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.17519999999999999</v>
       </c>
       <c r="T8" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.20439999999999997</v>
       </c>
       <c r="U8" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.2336</v>
       </c>
       <c r="V8" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.26279999999999998</v>
       </c>
       <c r="W8" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.29199999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AB8" s="2">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="AC8" s="7">
+        <v>0.27079999999999999</v>
+      </c>
+      <c r="AD8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE8">
+        <v>0.26344499999999998</v>
+      </c>
+      <c r="AF8">
+        <v>0.26344299999999998</v>
+      </c>
+      <c r="AG8">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="AH8" s="3">
+        <v>0.26298300000000002</v>
+      </c>
+      <c r="AI8">
+        <v>0.26449</v>
+      </c>
+      <c r="AJ8">
+        <v>0.26733499999999999</v>
+      </c>
+      <c r="AK8">
+        <v>0.27179999999999999</v>
+      </c>
+      <c r="AL8">
+        <v>0.24890000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -1175,47 +1442,81 @@
         <v>2.1830000000000002E-2</v>
       </c>
       <c r="N9">
-        <f t="shared" ref="N9:W9" si="15">$K$9*N2</f>
+        <f t="shared" ref="N9:W9" si="16">$K$9*N2</f>
         <v>4.3660000000000004E-2</v>
       </c>
       <c r="O9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6.5489999999999993E-2</v>
       </c>
       <c r="P9">
-        <f t="shared" ref="P9" si="16">$K$9*P2</f>
+        <f t="shared" ref="P9" si="17">$K$9*P2</f>
         <v>7.2039000000000006E-2</v>
       </c>
       <c r="Q9" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8.7320000000000009E-2</v>
       </c>
       <c r="R9" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.10915</v>
       </c>
       <c r="S9" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.13097999999999999</v>
       </c>
       <c r="T9" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.15280999999999997</v>
       </c>
       <c r="U9" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.17464000000000002</v>
       </c>
       <c r="V9" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.19647000000000001</v>
       </c>
       <c r="W9" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.21829999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AB9" s="2">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="AC9" s="7">
+        <v>0.21640000000000001</v>
+      </c>
+      <c r="AD9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE9">
+        <v>0.1961</v>
+      </c>
+      <c r="AF9">
+        <v>0.22242999999999999</v>
+      </c>
+      <c r="AG9">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AH9">
+        <v>0.19340499999999999</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>0.19328100000000001</v>
+      </c>
+      <c r="AJ9">
+        <v>0.19423000000000001</v>
+      </c>
+      <c r="AK9">
+        <v>0.19650000000000001</v>
+      </c>
+      <c r="AL9">
+        <v>0.2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <f t="shared" si="5"/>
         <v>8</v>
@@ -1247,47 +1548,81 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="N10">
-        <f t="shared" ref="N10:W10" si="17">$K$10*N2</f>
+        <f t="shared" ref="N10:W10" si="18">$K$10*N2</f>
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="O10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.3E-2</v>
       </c>
       <c r="P10">
-        <f t="shared" ref="P10" si="18">$K$10*P2</f>
+        <f t="shared" ref="P10" si="19">$K$10*P2</f>
         <v>6.93E-2</v>
       </c>
       <c r="Q10" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="R10" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.105</v>
       </c>
       <c r="S10" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.126</v>
       </c>
       <c r="T10" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.14699999999999999</v>
       </c>
       <c r="U10" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.16800000000000001</v>
       </c>
       <c r="V10" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.189</v>
       </c>
       <c r="W10" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.21</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="AB10" s="2">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="AC10" s="7">
+        <v>0.20380000000000001</v>
+      </c>
+      <c r="AD10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE10">
+        <v>0.194716</v>
+      </c>
+      <c r="AF10">
+        <v>0.19417000000000001</v>
+      </c>
+      <c r="AG10">
+        <v>0.193</v>
+      </c>
+      <c r="AH10">
+        <v>0.191746</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>0.191163</v>
+      </c>
+      <c r="AJ10">
+        <v>0.19120000000000001</v>
+      </c>
+      <c r="AK10">
+        <v>0.19203000000000001</v>
+      </c>
+      <c r="AL10">
+        <v>0.1943</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <f>B10+1</f>
         <v>9</v>
@@ -1319,47 +1654,115 @@
         <v>1.4080000000000002E-2</v>
       </c>
       <c r="N11">
-        <f t="shared" ref="N11:W11" si="19">$K$11*N2</f>
+        <f t="shared" ref="N11:W11" si="20">$K$11*N2</f>
         <v>2.8160000000000004E-2</v>
       </c>
       <c r="O11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>4.224E-2</v>
       </c>
       <c r="P11">
-        <f t="shared" ref="P11" si="20">$K$11*P2</f>
+        <f t="shared" ref="P11" si="21">$K$11*P2</f>
         <v>4.6464000000000005E-2</v>
       </c>
       <c r="Q11" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5.6320000000000009E-2</v>
       </c>
       <c r="R11" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7.0400000000000004E-2</v>
       </c>
       <c r="S11" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>8.448E-2</v>
       </c>
       <c r="T11" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.8559999999999995E-2</v>
       </c>
       <c r="U11" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.11264000000000002</v>
       </c>
       <c r="V11" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.12672</v>
       </c>
       <c r="W11" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.14080000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="AB11" s="2">
+        <f>AB10+1</f>
+        <v>9</v>
+      </c>
+      <c r="AC11" s="7">
+        <v>0.12570000000000001</v>
+      </c>
+      <c r="AD11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE11">
+        <v>0.12139999999999999</v>
+      </c>
+      <c r="AF11">
+        <v>0.12103999999999999</v>
+      </c>
+      <c r="AG11">
+        <v>0.1205</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>0.12019100000000001</v>
+      </c>
+      <c r="AI11">
+        <v>0.12034400000000001</v>
+      </c>
+      <c r="AJ11">
+        <v>0.12089999999999999</v>
+      </c>
+      <c r="AK11">
+        <v>0.122</v>
+      </c>
+      <c r="AL11">
+        <v>0.14180000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6">
+        <v>135000</v>
+      </c>
+      <c r="D17" s="6">
+        <v>145000</v>
+      </c>
+      <c r="E17" s="6">
+        <f>D17+10000</f>
+        <v>155000</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" ref="F17" si="22">E17+10000</f>
+        <v>165000</v>
+      </c>
+      <c r="G17" s="6">
+        <f t="shared" ref="G17" si="23">F17+10000</f>
+        <v>175000</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" ref="H17" si="24">G17+10000</f>
+        <v>185000</v>
+      </c>
+      <c r="K17" t="s">
+        <v>2</v>
+      </c>
       <c r="L17" t="s">
         <v>1</v>
       </c>
@@ -1369,359 +1772,992 @@
       <c r="N17" s="6">
         <v>0.2</v>
       </c>
-      <c r="O17" s="1">
+      <c r="O17" s="6">
         <v>0.3</v>
       </c>
-      <c r="P17" s="1">
+      <c r="P17" s="6">
         <v>0.33</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="Q17" s="6">
         <v>0.4</v>
       </c>
-      <c r="R17" s="1">
+      <c r="R17" s="6">
         <v>0.5</v>
       </c>
-      <c r="S17" s="1">
+      <c r="S17" s="6">
         <v>0.6</v>
       </c>
-      <c r="T17" s="1">
+      <c r="T17" s="6">
         <v>0.7</v>
       </c>
-      <c r="U17" s="1">
+      <c r="U17" s="6">
         <v>0.8</v>
       </c>
-      <c r="V17" s="1">
+      <c r="V17" s="6">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="18" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
+      <c r="W17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1.2783899999999999</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1.2798499999999999</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1.2808999999999999</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1.2811999999999999</v>
+      </c>
+      <c r="G18" s="7">
+        <v>1.2814000000000001</v>
+      </c>
+      <c r="H18" s="7">
+        <v>1.2812399999999999</v>
+      </c>
+      <c r="K18">
+        <v>1.25851</v>
+      </c>
       <c r="L18" s="2">
         <v>1</v>
       </c>
-      <c r="M18" s="7">
-        <v>1.0517000000000001</v>
-      </c>
-      <c r="N18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O18" s="4">
-        <v>1.0351999999999999</v>
-      </c>
-      <c r="P18" s="3">
-        <v>1.0343100000000001</v>
-      </c>
-      <c r="Q18" s="4">
-        <v>1.0345500000000001</v>
+      <c r="M18">
+        <f>$K$18*M17</f>
+        <v>0.12585100000000002</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ref="N18:W18" si="25">$K$18*N17</f>
+        <v>0.25170200000000004</v>
+      </c>
+      <c r="O18" s="3">
+        <f t="shared" si="25"/>
+        <v>0.37755299999999997</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="25"/>
+        <v>0.41530830000000002</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="25"/>
+        <v>0.50340400000000007</v>
       </c>
       <c r="R18">
-        <v>1.0388599999999999</v>
+        <f t="shared" si="25"/>
+        <v>0.62925500000000001</v>
       </c>
       <c r="S18">
-        <v>1.0471999999999999</v>
+        <f t="shared" si="25"/>
+        <v>0.75510599999999994</v>
       </c>
       <c r="T18">
-        <v>1.0601700000000001</v>
+        <f t="shared" si="25"/>
+        <v>0.88095699999999999</v>
       </c>
       <c r="U18">
-        <v>1.0808500000000001</v>
+        <f t="shared" si="25"/>
+        <v>1.0068080000000001</v>
       </c>
       <c r="V18">
-        <v>1.12018</v>
-      </c>
-    </row>
-    <row r="19" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="I19" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" s="3"/>
+        <f t="shared" si="25"/>
+        <v>1.1326590000000001</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="25"/>
+        <v>1.25851</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="AD18" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="AE18" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="AF18" s="6">
+        <v>0.33</v>
+      </c>
+      <c r="AG18" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="AH18" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AI18" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="AJ18" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="AK18" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="AL18" s="6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
+        <f>B18+1</f>
+        <v>2</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.72619999999999996</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0.72640000000000005</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0.7278</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0.72813499999999998</v>
+      </c>
+      <c r="H19" s="7">
+        <v>0.72812399999999999</v>
+      </c>
+      <c r="K19">
+        <v>0.78959999999999997</v>
+      </c>
       <c r="L19" s="2">
         <f>L18+1</f>
         <v>2</v>
       </c>
-      <c r="M19" s="7">
-        <v>0.63160000000000005</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O19" s="4">
-        <v>0.61319999999999997</v>
-      </c>
-      <c r="P19" s="3">
-        <v>0.61240000000000006</v>
-      </c>
-      <c r="Q19" s="4">
-        <v>0.61226999999999998</v>
+      <c r="M19">
+        <f>$K$19*M17</f>
+        <v>7.8960000000000002E-2</v>
+      </c>
+      <c r="N19">
+        <f t="shared" ref="N19:W19" si="26">$K$19*N17</f>
+        <v>0.15792</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="26"/>
+        <v>0.23687999999999998</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="26"/>
+        <v>0.26056800000000002</v>
+      </c>
+      <c r="Q19" s="3">
+        <f t="shared" si="26"/>
+        <v>0.31584000000000001</v>
       </c>
       <c r="R19">
-        <v>0.61481200000000003</v>
+        <f t="shared" si="26"/>
+        <v>0.39479999999999998</v>
       </c>
       <c r="S19">
-        <v>0.62050000000000005</v>
+        <f t="shared" si="26"/>
+        <v>0.47375999999999996</v>
       </c>
       <c r="T19">
-        <v>0.63029999999999997</v>
+        <f t="shared" si="26"/>
+        <v>0.55271999999999999</v>
       </c>
       <c r="U19">
-        <v>0.64649999999999996</v>
+        <f t="shared" si="26"/>
+        <v>0.63168000000000002</v>
       </c>
       <c r="V19">
-        <v>0.67700000000000005</v>
-      </c>
-    </row>
-    <row r="20" spans="9:22" x14ac:dyDescent="0.3">
+        <f t="shared" si="26"/>
+        <v>0.71063999999999994</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="26"/>
+        <v>0.78959999999999997</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="10"/>
+      <c r="AD19" s="11">
+        <v>1.0471999999999999</v>
+      </c>
+      <c r="AE19" s="12">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="AF19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG19" s="10">
+        <v>1.0467</v>
+      </c>
+      <c r="AH19" s="10">
+        <v>1.0526</v>
+      </c>
+      <c r="AI19" s="10">
+        <v>1.0622</v>
+      </c>
+      <c r="AJ19" s="10">
+        <v>1.0759000000000001</v>
+      </c>
+      <c r="AK19" s="10"/>
+      <c r="AL19" s="10"/>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
+        <f t="shared" ref="B20:B25" si="27">B19+1</f>
+        <v>3</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.56154999999999999</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.56194999999999995</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0.56379999999999997</v>
+      </c>
+      <c r="G20" s="7">
+        <v>0.5645</v>
+      </c>
+      <c r="H20" s="7">
+        <v>0.56479999999999997</v>
+      </c>
+      <c r="K20">
+        <v>0.58720000000000006</v>
+      </c>
       <c r="L20" s="2">
-        <f t="shared" ref="L20:L25" si="21">L19+1</f>
+        <f t="shared" ref="L20:L25" si="28">L19+1</f>
         <v>3</v>
       </c>
-      <c r="M20" s="7">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="N20" s="7" t="s">
-        <v>10</v>
+      <c r="M20">
+        <f>$K$20*M17</f>
+        <v>5.8720000000000008E-2</v>
+      </c>
+      <c r="N20">
+        <f t="shared" ref="N20:W20" si="29">$K$20*N17</f>
+        <v>0.11744000000000002</v>
       </c>
       <c r="O20">
-        <v>0.44340000000000002</v>
+        <f t="shared" si="29"/>
+        <v>0.17616000000000001</v>
       </c>
       <c r="P20">
-        <v>0.44112000000000001</v>
+        <f t="shared" si="29"/>
+        <v>0.19377600000000003</v>
       </c>
       <c r="Q20">
+        <f t="shared" si="29"/>
+        <v>0.23488000000000003</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="29"/>
+        <v>0.29360000000000003</v>
+      </c>
+      <c r="S20" s="3">
+        <f t="shared" si="29"/>
+        <v>0.35232000000000002</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="29"/>
+        <v>0.41104000000000002</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="29"/>
+        <v>0.46976000000000007</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="29"/>
+        <v>0.52848000000000006</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="29"/>
+        <v>0.58720000000000006</v>
+      </c>
+      <c r="AB20" s="2">
+        <f>AB19+1</f>
+        <v>2</v>
+      </c>
+      <c r="AC20" s="10"/>
+      <c r="AD20" s="11">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="AE20" s="10">
+        <v>0.58489999999999998</v>
+      </c>
+      <c r="AF20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG20" s="12">
+        <v>0.58420000000000005</v>
+      </c>
+      <c r="AH20" s="10">
+        <v>0.58720000000000006</v>
+      </c>
+      <c r="AI20" s="10">
+        <v>0.59389999999999998</v>
+      </c>
+      <c r="AJ20" s="10">
+        <v>0.60509999999999997</v>
+      </c>
+      <c r="AK20" s="10"/>
+      <c r="AL20" s="10"/>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="B21" s="2">
+        <f t="shared" si="27"/>
+        <v>4</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.56930000000000003</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.56930000000000003</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.56998000000000004</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0.57030000000000003</v>
+      </c>
+      <c r="G21" s="7">
+        <v>0.57669999999999999</v>
+      </c>
+      <c r="H21" s="7">
+        <v>0.57089999999999996</v>
+      </c>
+      <c r="K21">
+        <v>0.47620000000000001</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="28"/>
+        <v>4</v>
+      </c>
+      <c r="M21">
+        <f>$K$21*M17</f>
+        <v>4.7620000000000003E-2</v>
+      </c>
+      <c r="N21">
+        <f t="shared" ref="N21:W21" si="30">$K$21*N17</f>
+        <v>9.5240000000000005E-2</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="30"/>
+        <v>0.14285999999999999</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="30"/>
+        <v>0.15714600000000001</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="30"/>
+        <v>0.19048000000000001</v>
+      </c>
+      <c r="R21" s="3">
+        <f t="shared" si="30"/>
+        <v>0.23810000000000001</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="30"/>
+        <v>0.28571999999999997</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="30"/>
+        <v>0.33333999999999997</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="30"/>
+        <v>0.38096000000000002</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="30"/>
+        <v>0.42858000000000002</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="30"/>
+        <v>0.47620000000000001</v>
+      </c>
+      <c r="AB21" s="2">
+        <f t="shared" ref="AB21:AB26" si="31">AB20+1</f>
+        <v>3</v>
+      </c>
+      <c r="AC21" s="10"/>
+      <c r="AD21" s="11">
+        <v>0.44109999999999999</v>
+      </c>
+      <c r="AE21" s="11">
+        <v>0.43490000000000001</v>
+      </c>
+      <c r="AF21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG21" s="10">
+        <v>0.43120000000000003</v>
+      </c>
+      <c r="AH21" s="10">
+        <v>0.42830000000000001</v>
+      </c>
+      <c r="AI21" s="12">
+        <v>0.42720000000000002</v>
+      </c>
+      <c r="AJ21" s="10">
+        <v>0.4279</v>
+      </c>
+      <c r="AK21" s="10"/>
+      <c r="AL21" s="10"/>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
+        <f t="shared" si="27"/>
+        <v>5</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.35320000000000001</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0.35339999999999999</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0.35367999999999999</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0.35410000000000003</v>
+      </c>
+      <c r="G22" s="7">
+        <v>0.35439999999999999</v>
+      </c>
+      <c r="H22" s="7">
+        <v>0.35489999999999999</v>
+      </c>
+      <c r="K22">
+        <v>0.28322000000000003</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="28"/>
+        <v>5</v>
+      </c>
+      <c r="M22">
+        <f>$K$22*M17</f>
+        <v>2.8322000000000003E-2</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ref="N22:W22" si="32">$K$22*N17</f>
+        <v>5.6644000000000007E-2</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="32"/>
+        <v>8.4966E-2</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="32"/>
+        <v>9.3462600000000007E-2</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="32"/>
+        <v>0.11328800000000001</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="32"/>
+        <v>0.14161000000000001</v>
+      </c>
+      <c r="S22" s="3">
+        <f t="shared" si="32"/>
+        <v>0.169932</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="32"/>
+        <v>0.19825400000000001</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="32"/>
+        <v>0.22657600000000003</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="32"/>
+        <v>0.25489800000000001</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="32"/>
+        <v>0.28322000000000003</v>
+      </c>
+      <c r="AB22" s="2">
+        <f t="shared" si="31"/>
+        <v>4</v>
+      </c>
+      <c r="AC22" s="10"/>
+      <c r="AD22" s="11">
+        <v>0.4415</v>
+      </c>
+      <c r="AE22" s="10">
         <v>0.43790000000000001</v>
       </c>
-      <c r="R20">
-        <v>0.435172</v>
-      </c>
-      <c r="S20" s="3">
-        <v>0.43409999999999999</v>
-      </c>
-      <c r="T20">
-        <v>0.43530000000000002</v>
-      </c>
-      <c r="U20">
-        <v>0.43890000000000001</v>
-      </c>
-      <c r="V20">
-        <v>0.44790000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="L21" s="2">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="M21" s="7">
-        <v>0.47339999999999999</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O21">
-        <v>0.45989999999999998</v>
-      </c>
-      <c r="P21">
-        <v>0.45856000000000002</v>
-      </c>
-      <c r="Q21">
-        <v>0.45660000000000001</v>
-      </c>
-      <c r="R21">
-        <v>0.45506799999999997</v>
-      </c>
-      <c r="S21" s="3">
-        <v>0.45450000000000002</v>
-      </c>
-      <c r="T21">
-        <v>0.45469999999999999</v>
-      </c>
-      <c r="U21">
-        <v>0.45579999999999998</v>
-      </c>
-      <c r="V21">
-        <v>0.45800000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="L22" s="2">
-        <f t="shared" si="21"/>
+      <c r="AF22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG22" s="10">
+        <v>0.43590000000000001</v>
+      </c>
+      <c r="AH22" s="12">
+        <v>0.43580000000000002</v>
+      </c>
+      <c r="AI22" s="10">
+        <v>0.43669999999999998</v>
+      </c>
+      <c r="AJ22" s="10">
+        <v>0.43580000000000002</v>
+      </c>
+      <c r="AK22" s="10"/>
+      <c r="AL22" s="10"/>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="B23" s="2">
+        <f t="shared" si="27"/>
+        <v>6</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="D23" s="7">
+        <v>0.32569999999999999</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0.32599</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0.32586999999999999</v>
+      </c>
+      <c r="G23" s="7">
+        <v>0.32644000000000001</v>
+      </c>
+      <c r="H23" s="7">
+        <v>0.32690000000000002</v>
+      </c>
+      <c r="K23">
+        <v>0.26523999999999998</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="28"/>
+        <v>6</v>
+      </c>
+      <c r="M23">
+        <f>$K$23*M17</f>
+        <v>2.6523999999999999E-2</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ref="N23:W23" si="33">$K$23*N17</f>
+        <v>5.3047999999999998E-2</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="33"/>
+        <v>7.957199999999999E-2</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="33"/>
+        <v>8.7529200000000001E-2</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="33"/>
+        <v>0.106096</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="33"/>
+        <v>0.13261999999999999</v>
+      </c>
+      <c r="S23" s="3">
+        <f t="shared" si="33"/>
+        <v>0.15914399999999998</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="33"/>
+        <v>0.18566799999999997</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="33"/>
+        <v>0.21219199999999999</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="33"/>
+        <v>0.23871599999999998</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="33"/>
+        <v>0.26523999999999998</v>
+      </c>
+      <c r="AB23" s="2">
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
-      <c r="M22" s="7">
-        <v>0.31059999999999999</v>
-      </c>
-      <c r="N22" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O22">
-        <v>0.29770000000000002</v>
-      </c>
-      <c r="P22">
-        <v>0.29703000000000002</v>
-      </c>
-      <c r="Q22">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="R22" s="3">
-        <v>0.29538900000000001</v>
-      </c>
-      <c r="S22">
-        <v>0.29565000000000002</v>
-      </c>
-      <c r="T22">
-        <v>0.29670000000000002</v>
-      </c>
-      <c r="U22">
-        <v>0.29899999999999999</v>
-      </c>
-      <c r="V22">
-        <v>0.3034</v>
-      </c>
-    </row>
-    <row r="23" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="L23" s="2">
-        <f t="shared" si="21"/>
+      <c r="AC23" s="10"/>
+      <c r="AD23" s="11">
+        <v>0.26540000000000002</v>
+      </c>
+      <c r="AE23" s="11">
+        <v>0.26219999999999999</v>
+      </c>
+      <c r="AF23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG23" s="10">
+        <v>0.25950000000000001</v>
+      </c>
+      <c r="AH23" s="10">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="AI23" s="12">
+        <v>0.25729999999999997</v>
+      </c>
+      <c r="AJ23" s="10">
+        <v>0.2576</v>
+      </c>
+      <c r="AK23" s="10"/>
+      <c r="AL23" s="10"/>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
+        <f t="shared" si="27"/>
+        <v>7</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.23780000000000001</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0.23769999999999999</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.23777999999999999</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0.23780000000000001</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0.2379</v>
+      </c>
+      <c r="H24" s="7">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="K24">
+        <v>0.21060000000000001</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="28"/>
+        <v>7</v>
+      </c>
+      <c r="M24">
+        <f>$K$24*M17</f>
+        <v>2.1060000000000002E-2</v>
+      </c>
+      <c r="N24">
+        <f t="shared" ref="N24:W24" si="34">$K$24*N17</f>
+        <v>4.2120000000000005E-2</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="34"/>
+        <v>6.318E-2</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="34"/>
+        <v>6.9498000000000004E-2</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="34"/>
+        <v>8.4240000000000009E-2</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="34"/>
+        <v>0.1053</v>
+      </c>
+      <c r="S24" s="3">
+        <f t="shared" si="34"/>
+        <v>0.12636</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="34"/>
+        <v>0.14742</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="34"/>
+        <v>0.16848000000000002</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="34"/>
+        <v>0.18954000000000001</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="34"/>
+        <v>0.21060000000000001</v>
+      </c>
+      <c r="AB24" s="2">
+        <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="M23" s="7">
-        <v>0.27079999999999999</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O23">
-        <v>0.26344499999999998</v>
-      </c>
-      <c r="P23">
-        <v>0.26344299999999998</v>
-      </c>
-      <c r="Q23">
-        <v>0.26200000000000001</v>
-      </c>
-      <c r="R23" s="3">
-        <v>0.26298300000000002</v>
-      </c>
-      <c r="S23">
-        <v>0.26449</v>
-      </c>
-      <c r="T23">
-        <v>0.26733499999999999</v>
-      </c>
-      <c r="U23">
-        <v>0.27179999999999999</v>
-      </c>
-      <c r="V23">
-        <v>0.24890000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="L24" s="2">
-        <f t="shared" si="21"/>
+      <c r="AC24" s="10"/>
+      <c r="AD24" s="11">
+        <v>0.25419999999999998</v>
+      </c>
+      <c r="AE24" s="10">
+        <v>0.2505</v>
+      </c>
+      <c r="AF24" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG24" s="10">
+        <v>0.24809999999999999</v>
+      </c>
+      <c r="AH24" s="10">
+        <v>0.247</v>
+      </c>
+      <c r="AI24" s="12">
+        <v>0.2467</v>
+      </c>
+      <c r="AJ24" s="10">
+        <v>0.24729999999999999</v>
+      </c>
+      <c r="AK24" s="10"/>
+      <c r="AL24" s="10"/>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="B25" s="2">
+        <f t="shared" si="27"/>
+        <v>8</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.22770000000000001</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0.2281</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0.22839999999999999</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0.2286</v>
+      </c>
+      <c r="G25" s="7">
+        <v>0.22869999999999999</v>
+      </c>
+      <c r="H25" s="7">
+        <v>0.2288</v>
+      </c>
+      <c r="K25">
+        <v>0.18725</v>
+      </c>
+      <c r="L25" s="2">
+        <f t="shared" si="28"/>
+        <v>8</v>
+      </c>
+      <c r="M25">
+        <f>$K$25*M17</f>
+        <v>1.8725000000000002E-2</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ref="N25:W25" si="35">$K$25*N17</f>
+        <v>3.7450000000000004E-2</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="35"/>
+        <v>5.6174999999999996E-2</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="35"/>
+        <v>6.17925E-2</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="35"/>
+        <v>7.4900000000000008E-2</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="35"/>
+        <v>9.3625E-2</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="35"/>
+        <v>0.11234999999999999</v>
+      </c>
+      <c r="T25" s="3">
+        <f t="shared" si="35"/>
+        <v>0.131075</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="35"/>
+        <v>0.14980000000000002</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="35"/>
+        <v>0.16852500000000001</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="35"/>
+        <v>0.18725</v>
+      </c>
+      <c r="AB25" s="2">
+        <f t="shared" si="31"/>
         <v>7</v>
       </c>
-      <c r="M24" s="7">
-        <v>0.21640000000000001</v>
-      </c>
-      <c r="N24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O24">
-        <v>0.1961</v>
-      </c>
-      <c r="P24">
-        <v>0.22242999999999999</v>
-      </c>
-      <c r="Q24">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="R24">
-        <v>0.19340499999999999</v>
-      </c>
-      <c r="S24" s="3">
-        <v>0.19328100000000001</v>
-      </c>
-      <c r="T24">
-        <v>0.19423000000000001</v>
-      </c>
-      <c r="U24">
-        <v>0.19650000000000001</v>
-      </c>
-      <c r="V24">
-        <v>0.2014</v>
-      </c>
-    </row>
-    <row r="25" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="L25" s="2">
-        <f t="shared" si="21"/>
-        <v>8</v>
-      </c>
-      <c r="M25" s="7">
-        <v>0.20380000000000001</v>
-      </c>
-      <c r="N25" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O25">
-        <v>0.194716</v>
-      </c>
-      <c r="P25">
-        <v>0.19417000000000001</v>
-      </c>
-      <c r="Q25">
-        <v>0.193</v>
-      </c>
-      <c r="R25">
-        <v>0.191746</v>
-      </c>
-      <c r="S25" s="3">
-        <v>0.191163</v>
-      </c>
-      <c r="T25">
-        <v>0.19120000000000001</v>
-      </c>
-      <c r="U25">
-        <v>0.19203000000000001</v>
-      </c>
-      <c r="V25">
-        <v>0.1943</v>
-      </c>
-    </row>
-    <row r="26" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="AC25" s="10"/>
+      <c r="AD25" s="11">
+        <v>0.18859999999999999</v>
+      </c>
+      <c r="AE25" s="11">
+        <v>0.18629999999999999</v>
+      </c>
+      <c r="AF25" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG25" s="10">
+        <v>0.18509999999999999</v>
+      </c>
+      <c r="AH25" s="10">
+        <v>0.18390000000000001</v>
+      </c>
+      <c r="AI25" s="12">
+        <v>0.18329999999999999</v>
+      </c>
+      <c r="AJ25" s="10">
+        <v>0.18360000000000001</v>
+      </c>
+      <c r="AK25" s="10"/>
+      <c r="AL25" s="10"/>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="B26" s="2">
+        <f>B25+1</f>
+        <v>9</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.1293</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0.1288</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0.12892999999999999</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0.12902</v>
+      </c>
+      <c r="G26" s="7">
+        <v>0.12909999999999999</v>
+      </c>
+      <c r="H26" s="7">
+        <v>0.12920000000000001</v>
+      </c>
+      <c r="K26">
+        <v>0.12507699999999999</v>
+      </c>
       <c r="L26" s="2">
         <f>L25+1</f>
         <v>9</v>
       </c>
-      <c r="M26" s="7">
-        <v>0.12570000000000001</v>
-      </c>
-      <c r="N26" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O26">
-        <v>0.12139999999999999</v>
+      <c r="M26">
+        <f>$K$26*M17</f>
+        <v>1.25077E-2</v>
+      </c>
+      <c r="N26">
+        <f t="shared" ref="N26:W26" si="36">$K$26*N17</f>
+        <v>2.50154E-2</v>
+      </c>
+      <c r="O26" s="3">
+        <f t="shared" si="36"/>
+        <v>3.7523099999999997E-2</v>
       </c>
       <c r="P26">
-        <v>0.12103999999999999</v>
+        <f t="shared" si="36"/>
+        <v>4.1275409999999998E-2</v>
       </c>
       <c r="Q26">
-        <v>0.1205</v>
-      </c>
-      <c r="R26" s="3">
-        <v>0.12019100000000001</v>
+        <f t="shared" si="36"/>
+        <v>5.00308E-2</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="36"/>
+        <v>6.2538499999999997E-2</v>
       </c>
       <c r="S26">
-        <v>0.12034400000000001</v>
+        <f t="shared" si="36"/>
+        <v>7.5046199999999993E-2</v>
       </c>
       <c r="T26">
-        <v>0.12089999999999999</v>
+        <f t="shared" si="36"/>
+        <v>8.755389999999999E-2</v>
       </c>
       <c r="U26">
-        <v>0.122</v>
+        <f t="shared" si="36"/>
+        <v>0.1000616</v>
       </c>
       <c r="V26">
-        <v>0.14180000000000001</v>
-      </c>
+        <f t="shared" si="36"/>
+        <v>0.1125693</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="36"/>
+        <v>0.12507699999999999</v>
+      </c>
+      <c r="AB26" s="2">
+        <f t="shared" si="31"/>
+        <v>8</v>
+      </c>
+      <c r="AC26" s="10"/>
+      <c r="AD26" s="11">
+        <v>0.185</v>
+      </c>
+      <c r="AE26" s="11">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="AF26" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG26" s="10">
+        <v>0.1749</v>
+      </c>
+      <c r="AH26" s="10">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="AI26" s="10">
+        <v>0.1734</v>
+      </c>
+      <c r="AJ26" s="12">
+        <v>0.17319999999999999</v>
+      </c>
+      <c r="AK26" s="10"/>
+      <c r="AL26" s="10"/>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AB27" s="2">
+        <f>AB26+1</f>
+        <v>9</v>
+      </c>
+      <c r="AC27" s="10"/>
+      <c r="AD27" s="11">
+        <v>0.10081</v>
+      </c>
+      <c r="AE27" s="12">
+        <v>0.1008</v>
+      </c>
+      <c r="AF27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG27" s="10">
+        <v>0.1008</v>
+      </c>
+      <c r="AH27" s="10">
+        <v>0.1014</v>
+      </c>
+      <c r="AI27" s="10">
+        <v>0.1023</v>
+      </c>
+      <c r="AJ27" s="10">
+        <v>0.10366</v>
+      </c>
+      <c r="AK27" s="10"/>
+      <c r="AL27" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adjusting preprocessing notebook for adjusted PCA
next step is doing interpolation for each area with new PCA
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/optimal_nugget_range_value.xlsx
+++ b/_INTERPOLATION/optimal_nugget_range_value.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\python_map\New\Vistelius_1995_OCR\_INTERPOLATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF01984-4E2E-460F-8673-E6D4F0057191}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628A541C-3B87-4885-AD99-9084AC5042DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{B3A2F8EB-B1AE-45BB-BB45-54B64F4D81FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{B3A2F8EB-B1AE-45BB-BB45-54B64F4D81FD}"/>
   </bookViews>
   <sheets>
     <sheet name="# control points" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="area 3" sheetId="3" r:id="rId4"/>
     <sheet name="area 4" sheetId="4" r:id="rId5"/>
     <sheet name="area 5" sheetId="5" r:id="rId6"/>
-    <sheet name="area6" sheetId="8" r:id="rId7"/>
+    <sheet name="area2_a" sheetId="8" r:id="rId7"/>
+    <sheet name="area2_b" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="28">
   <si>
     <t>range</t>
   </si>
@@ -118,14 +119,20 @@
   <si>
     <t>new boundaies</t>
   </si>
+  <si>
+    <t>spherical model = best model here!?</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -231,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -247,13 +254,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -9907,8 +9919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D51598-43C8-43C8-B0AF-4826DB32F76D}">
   <dimension ref="A2:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10829,9 +10841,6 @@
       </c>
     </row>
     <row r="24" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="I24" t="s">
-        <v>8</v>
-      </c>
       <c r="L24" s="2">
         <f t="shared" si="12"/>
         <v>7</v>
@@ -10865,9 +10874,6 @@
       </c>
     </row>
     <row r="25" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="I25" t="s">
-        <v>9</v>
-      </c>
       <c r="L25" s="2">
         <f t="shared" si="12"/>
         <v>8</v>
@@ -10936,4 +10942,1583 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1A3264-3A61-4411-A092-3122019449F9}">
+  <dimension ref="A2:V38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="7" width="11.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" style="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="17">
+        <v>75000</v>
+      </c>
+      <c r="D2" s="17">
+        <f>C2+5000</f>
+        <v>80000</v>
+      </c>
+      <c r="E2" s="17">
+        <f t="shared" ref="E2:H2" si="0">D2+5000</f>
+        <v>85000</v>
+      </c>
+      <c r="F2" s="17">
+        <f t="shared" si="0"/>
+        <v>90000</v>
+      </c>
+      <c r="G2" s="17">
+        <f t="shared" si="0"/>
+        <v>95000</v>
+      </c>
+      <c r="H2" s="17">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="O2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="P2" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R2" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="S2" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="T2" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="U2" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="V2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="26">
+        <v>2.7652000000000001</v>
+      </c>
+      <c r="D3" s="26">
+        <v>2.7642000000000002</v>
+      </c>
+      <c r="E3" s="26">
+        <v>2.7650000000000001</v>
+      </c>
+      <c r="F3" s="26">
+        <v>2.7681</v>
+      </c>
+      <c r="G3" s="26">
+        <v>2.7696999999999998</v>
+      </c>
+      <c r="H3" s="26">
+        <v>2.7719</v>
+      </c>
+      <c r="K3" s="16">
+        <v>1.7316</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" s="7">
+        <f>$K$3*M2</f>
+        <v>0.17316000000000001</v>
+      </c>
+      <c r="N3" s="7">
+        <f t="shared" ref="N3:V3" si="1">$K$3*N2</f>
+        <v>0.34632000000000002</v>
+      </c>
+      <c r="O3" s="7">
+        <f t="shared" si="1"/>
+        <v>0.51947999999999994</v>
+      </c>
+      <c r="P3" s="7">
+        <f t="shared" si="1"/>
+        <v>0.69264000000000003</v>
+      </c>
+      <c r="Q3" s="7">
+        <f t="shared" si="1"/>
+        <v>0.86580000000000001</v>
+      </c>
+      <c r="R3" s="7">
+        <f t="shared" si="1"/>
+        <v>1.0389599999999999</v>
+      </c>
+      <c r="S3" s="7">
+        <f t="shared" si="1"/>
+        <v>1.2121199999999999</v>
+      </c>
+      <c r="T3" s="7">
+        <f t="shared" si="1"/>
+        <v>1.3852800000000001</v>
+      </c>
+      <c r="U3" s="7">
+        <f t="shared" si="1"/>
+        <v>1.55844</v>
+      </c>
+      <c r="V3" s="7">
+        <f t="shared" si="1"/>
+        <v>1.7316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <f>B3+1</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="26">
+        <v>1.1156999999999999</v>
+      </c>
+      <c r="D4" s="26">
+        <v>1.1153999999999999</v>
+      </c>
+      <c r="E4" s="26">
+        <v>1.1168</v>
+      </c>
+      <c r="F4" s="26">
+        <v>1.1165</v>
+      </c>
+      <c r="G4" s="26">
+        <v>1.1180000000000001</v>
+      </c>
+      <c r="H4" s="26">
+        <v>1.1187</v>
+      </c>
+      <c r="K4" s="16">
+        <v>1.0281100000000001</v>
+      </c>
+      <c r="L4" s="2">
+        <f>L3+1</f>
+        <v>2</v>
+      </c>
+      <c r="M4" s="7">
+        <f>$K$4*M2</f>
+        <v>0.10281100000000001</v>
+      </c>
+      <c r="N4" s="7">
+        <f t="shared" ref="N4:V4" si="2">$K$4*N2</f>
+        <v>0.20562200000000003</v>
+      </c>
+      <c r="O4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.30843300000000001</v>
+      </c>
+      <c r="P4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.41124400000000005</v>
+      </c>
+      <c r="Q4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.51405500000000004</v>
+      </c>
+      <c r="R4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.61686600000000003</v>
+      </c>
+      <c r="S4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.71967700000000001</v>
+      </c>
+      <c r="T4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.82248800000000011</v>
+      </c>
+      <c r="U4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.92529900000000009</v>
+      </c>
+      <c r="V4" s="7">
+        <f t="shared" si="2"/>
+        <v>1.0281100000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <f t="shared" ref="B5:B10" si="3">B4+1</f>
+        <v>3</v>
+      </c>
+      <c r="C5" s="26">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="D5" s="26">
+        <v>0.79930000000000001</v>
+      </c>
+      <c r="E5" s="26">
+        <v>0.80020000000000002</v>
+      </c>
+      <c r="F5" s="26">
+        <v>0.79930000000000001</v>
+      </c>
+      <c r="G5" s="26">
+        <v>0.80049999999999999</v>
+      </c>
+      <c r="H5" s="26">
+        <v>0.80059999999999998</v>
+      </c>
+      <c r="K5" s="16">
+        <v>0.65720000000000001</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" ref="L5:L10" si="4">L4+1</f>
+        <v>3</v>
+      </c>
+      <c r="M5" s="7">
+        <f>$K$5*M2</f>
+        <v>6.5720000000000001E-2</v>
+      </c>
+      <c r="N5" s="7">
+        <f t="shared" ref="N5:V5" si="5">$K$5*N2</f>
+        <v>0.13144</v>
+      </c>
+      <c r="O5" s="7">
+        <f t="shared" si="5"/>
+        <v>0.19716</v>
+      </c>
+      <c r="P5" s="7">
+        <f t="shared" si="5"/>
+        <v>0.26288</v>
+      </c>
+      <c r="Q5" s="7">
+        <f>$K$5*Q2</f>
+        <v>0.3286</v>
+      </c>
+      <c r="R5" s="7">
+        <f t="shared" si="5"/>
+        <v>0.39432</v>
+      </c>
+      <c r="S5" s="7">
+        <f t="shared" si="5"/>
+        <v>0.46003999999999995</v>
+      </c>
+      <c r="T5" s="7">
+        <f t="shared" si="5"/>
+        <v>0.52576000000000001</v>
+      </c>
+      <c r="U5" s="7">
+        <f t="shared" si="5"/>
+        <v>0.59148000000000001</v>
+      </c>
+      <c r="V5" s="7">
+        <f t="shared" si="5"/>
+        <v>0.65720000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="C6" s="26">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="D6" s="26">
+        <v>0.7903</v>
+      </c>
+      <c r="E6" s="26">
+        <v>0.79120000000000001</v>
+      </c>
+      <c r="F6" s="26">
+        <v>0.7913</v>
+      </c>
+      <c r="G6" s="26">
+        <v>0.79149999999999998</v>
+      </c>
+      <c r="H6" s="26">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0.57330000000000003</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="M6" s="7">
+        <f>$K$6*M2</f>
+        <v>5.7330000000000006E-2</v>
+      </c>
+      <c r="N6" s="7">
+        <f t="shared" ref="N6:V6" si="6">$K$6*N2</f>
+        <v>0.11466000000000001</v>
+      </c>
+      <c r="O6" s="7">
+        <f t="shared" si="6"/>
+        <v>0.17199</v>
+      </c>
+      <c r="P6" s="7">
+        <f t="shared" si="6"/>
+        <v>0.22932000000000002</v>
+      </c>
+      <c r="Q6" s="7">
+        <f t="shared" si="6"/>
+        <v>0.28665000000000002</v>
+      </c>
+      <c r="R6" s="7">
+        <f t="shared" si="6"/>
+        <v>0.34398000000000001</v>
+      </c>
+      <c r="S6" s="8">
+        <f t="shared" si="6"/>
+        <v>0.40131</v>
+      </c>
+      <c r="T6" s="7">
+        <f t="shared" si="6"/>
+        <v>0.45864000000000005</v>
+      </c>
+      <c r="U6" s="7">
+        <f t="shared" si="6"/>
+        <v>0.51597000000000004</v>
+      </c>
+      <c r="V6" s="7">
+        <f t="shared" si="6"/>
+        <v>0.57330000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="C7" s="26">
+        <v>0.57379999999999998</v>
+      </c>
+      <c r="D7" s="26">
+        <v>0.57420000000000004</v>
+      </c>
+      <c r="E7" s="26">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="F7" s="26">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="G7" s="26">
+        <v>0.57530000000000003</v>
+      </c>
+      <c r="H7" s="26">
+        <v>0.57520000000000004</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0.49590000000000001</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="M7" s="7">
+        <f>$K$7*M2</f>
+        <v>4.9590000000000002E-2</v>
+      </c>
+      <c r="N7" s="7">
+        <f t="shared" ref="N7:V7" si="7">$K$7*N2</f>
+        <v>9.9180000000000004E-2</v>
+      </c>
+      <c r="O7" s="7">
+        <f t="shared" si="7"/>
+        <v>0.14876999999999999</v>
+      </c>
+      <c r="P7" s="7">
+        <f>$K$7*P2</f>
+        <v>0.19836000000000001</v>
+      </c>
+      <c r="Q7" s="7">
+        <f t="shared" si="7"/>
+        <v>0.24795</v>
+      </c>
+      <c r="R7" s="7">
+        <f t="shared" si="7"/>
+        <v>0.29753999999999997</v>
+      </c>
+      <c r="S7" s="7">
+        <f t="shared" si="7"/>
+        <v>0.34712999999999999</v>
+      </c>
+      <c r="T7" s="7">
+        <f t="shared" si="7"/>
+        <v>0.39672000000000002</v>
+      </c>
+      <c r="U7" s="7">
+        <f t="shared" si="7"/>
+        <v>0.44631000000000004</v>
+      </c>
+      <c r="V7" s="7">
+        <f t="shared" si="7"/>
+        <v>0.49590000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="C8" s="26">
+        <v>0.5645</v>
+      </c>
+      <c r="D8" s="26">
+        <v>0.56559999999999999</v>
+      </c>
+      <c r="E8" s="26">
+        <v>0.5655</v>
+      </c>
+      <c r="F8" s="26">
+        <v>0.56610000000000005</v>
+      </c>
+      <c r="G8" s="26">
+        <v>0.56569999999999998</v>
+      </c>
+      <c r="H8" s="26">
+        <v>0.56610000000000005</v>
+      </c>
+      <c r="K8" s="16">
+        <v>0.4491</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="M8" s="7">
+        <f>$K$8*M2</f>
+        <v>4.4910000000000005E-2</v>
+      </c>
+      <c r="N8" s="7">
+        <f t="shared" ref="N8:V8" si="8">$K$8*N2</f>
+        <v>8.9820000000000011E-2</v>
+      </c>
+      <c r="O8" s="7">
+        <f t="shared" si="8"/>
+        <v>0.13472999999999999</v>
+      </c>
+      <c r="P8" s="7">
+        <f t="shared" si="8"/>
+        <v>0.17964000000000002</v>
+      </c>
+      <c r="Q8" s="7">
+        <f t="shared" si="8"/>
+        <v>0.22455</v>
+      </c>
+      <c r="R8" s="7">
+        <f t="shared" si="8"/>
+        <v>0.26945999999999998</v>
+      </c>
+      <c r="S8" s="7">
+        <f t="shared" si="8"/>
+        <v>0.31436999999999998</v>
+      </c>
+      <c r="T8" s="7">
+        <f t="shared" si="8"/>
+        <v>0.35928000000000004</v>
+      </c>
+      <c r="U8" s="7">
+        <f t="shared" si="8"/>
+        <v>0.40418999999999999</v>
+      </c>
+      <c r="V8" s="7">
+        <f t="shared" si="8"/>
+        <v>0.4491</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0.43309999999999998</v>
+      </c>
+      <c r="D9" s="26">
+        <v>0.43340000000000001</v>
+      </c>
+      <c r="E9" s="26">
+        <v>0.43369999999999997</v>
+      </c>
+      <c r="F9" s="26">
+        <v>0.43340000000000001</v>
+      </c>
+      <c r="G9" s="26">
+        <v>0.43369999999999997</v>
+      </c>
+      <c r="H9" s="26">
+        <v>0.43390000000000001</v>
+      </c>
+      <c r="K9" s="16">
+        <v>0.27679999999999999</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="M9" s="7">
+        <f>$K$9*M2</f>
+        <v>2.768E-2</v>
+      </c>
+      <c r="N9" s="7">
+        <f t="shared" ref="N9:V9" si="9">$K$9*N2</f>
+        <v>5.5359999999999999E-2</v>
+      </c>
+      <c r="O9" s="7">
+        <f t="shared" si="9"/>
+        <v>8.3039999999999989E-2</v>
+      </c>
+      <c r="P9" s="7">
+        <f t="shared" si="9"/>
+        <v>0.11072</v>
+      </c>
+      <c r="Q9" s="7">
+        <f t="shared" si="9"/>
+        <v>0.1384</v>
+      </c>
+      <c r="R9" s="7">
+        <f>$K$9*R2</f>
+        <v>0.16607999999999998</v>
+      </c>
+      <c r="S9" s="7">
+        <f t="shared" si="9"/>
+        <v>0.19375999999999999</v>
+      </c>
+      <c r="T9" s="7">
+        <f t="shared" si="9"/>
+        <v>0.22144</v>
+      </c>
+      <c r="U9" s="7">
+        <f t="shared" si="9"/>
+        <v>0.24912000000000001</v>
+      </c>
+      <c r="V9" s="7">
+        <f t="shared" si="9"/>
+        <v>0.27679999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="26">
+        <v>0.31609999999999999</v>
+      </c>
+      <c r="D10" s="26">
+        <v>0.31659999999999999</v>
+      </c>
+      <c r="E10" s="26">
+        <v>0.31709999999999999</v>
+      </c>
+      <c r="F10" s="26">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="G10" s="26">
+        <v>0.3175</v>
+      </c>
+      <c r="H10" s="26">
+        <v>0.31769999999999998</v>
+      </c>
+      <c r="K10" s="16">
+        <v>0.23930000000000001</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="M10" s="7">
+        <f>$K$10*M2</f>
+        <v>2.3930000000000003E-2</v>
+      </c>
+      <c r="N10" s="7">
+        <f t="shared" ref="N10:V10" si="10">$K$10*N2</f>
+        <v>4.7860000000000007E-2</v>
+      </c>
+      <c r="O10" s="7">
+        <f t="shared" si="10"/>
+        <v>7.1790000000000007E-2</v>
+      </c>
+      <c r="P10" s="7">
+        <f t="shared" si="10"/>
+        <v>9.5720000000000013E-2</v>
+      </c>
+      <c r="Q10" s="7">
+        <f t="shared" si="10"/>
+        <v>0.11965000000000001</v>
+      </c>
+      <c r="R10" s="7">
+        <f t="shared" si="10"/>
+        <v>0.14358000000000001</v>
+      </c>
+      <c r="S10" s="7">
+        <f>$K$10*S2</f>
+        <v>0.16750999999999999</v>
+      </c>
+      <c r="T10" s="7">
+        <f t="shared" si="10"/>
+        <v>0.19144000000000003</v>
+      </c>
+      <c r="U10" s="7">
+        <f t="shared" si="10"/>
+        <v>0.21537000000000001</v>
+      </c>
+      <c r="V10" s="7">
+        <f t="shared" si="10"/>
+        <v>0.23930000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <f>B10+1</f>
+        <v>9</v>
+      </c>
+      <c r="C11" s="26">
+        <v>0.25540000000000002</v>
+      </c>
+      <c r="D11" s="26">
+        <v>0.25569999999999998</v>
+      </c>
+      <c r="E11" s="26">
+        <v>0.25580000000000003</v>
+      </c>
+      <c r="F11" s="26">
+        <v>0.25590000000000002</v>
+      </c>
+      <c r="G11" s="26">
+        <v>0.25609999999999999</v>
+      </c>
+      <c r="H11" s="26">
+        <v>0.25629999999999997</v>
+      </c>
+      <c r="K11" s="16">
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="L11" s="2">
+        <f>L10+1</f>
+        <v>9</v>
+      </c>
+      <c r="M11" s="7">
+        <f>$K$11*M2</f>
+        <v>1.8679999999999999E-2</v>
+      </c>
+      <c r="N11" s="7">
+        <f t="shared" ref="N11:V11" si="11">$K$11*N2</f>
+        <v>3.7359999999999997E-2</v>
+      </c>
+      <c r="O11" s="7">
+        <f t="shared" si="11"/>
+        <v>5.604E-2</v>
+      </c>
+      <c r="P11" s="7">
+        <f>$K$11*P2</f>
+        <v>7.4719999999999995E-2</v>
+      </c>
+      <c r="Q11" s="7">
+        <f t="shared" si="11"/>
+        <v>9.3399999999999997E-2</v>
+      </c>
+      <c r="R11" s="7">
+        <f t="shared" si="11"/>
+        <v>0.11208</v>
+      </c>
+      <c r="S11" s="7">
+        <f t="shared" si="11"/>
+        <v>0.13075999999999999</v>
+      </c>
+      <c r="T11" s="7">
+        <f t="shared" si="11"/>
+        <v>0.14943999999999999</v>
+      </c>
+      <c r="U11" s="7">
+        <f t="shared" si="11"/>
+        <v>0.16811999999999999</v>
+      </c>
+      <c r="V11" s="7">
+        <f t="shared" si="11"/>
+        <v>0.18679999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C13" s="25">
+        <v>25000</v>
+      </c>
+      <c r="D13" s="24">
+        <f>C13+5000</f>
+        <v>30000</v>
+      </c>
+      <c r="E13" s="24">
+        <f t="shared" ref="E13:G13" si="12">D13+5000</f>
+        <v>35000</v>
+      </c>
+      <c r="F13" s="24">
+        <f t="shared" si="12"/>
+        <v>40000</v>
+      </c>
+      <c r="G13" s="24">
+        <v>50000</v>
+      </c>
+      <c r="H13" s="24">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="22">
+        <v>2.6520000000000001</v>
+      </c>
+      <c r="D14" s="16">
+        <v>2.6783000000000001</v>
+      </c>
+      <c r="E14" s="16">
+        <v>2.7153999999999998</v>
+      </c>
+      <c r="F14" s="16">
+        <v>2.7299000000000002</v>
+      </c>
+      <c r="G14" s="15">
+        <v>2.7410000000000001</v>
+      </c>
+      <c r="H14" s="15">
+        <v>2.7498999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B15" s="2">
+        <f>B14+1</f>
+        <v>2</v>
+      </c>
+      <c r="C15" s="16">
+        <v>1.0851999999999999</v>
+      </c>
+      <c r="D15" s="22">
+        <v>1.0840700000000001</v>
+      </c>
+      <c r="E15" s="16">
+        <v>1.101</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1.10022</v>
+      </c>
+      <c r="G15" s="15">
+        <v>1.1048</v>
+      </c>
+      <c r="H15" s="15">
+        <v>1.1086</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B16" s="2">
+        <f t="shared" ref="B16:B21" si="13">B15+1</f>
+        <v>3</v>
+      </c>
+      <c r="C16" s="22">
+        <v>0.76929999999999998</v>
+      </c>
+      <c r="D16" s="16">
+        <v>0.77880000000000005</v>
+      </c>
+      <c r="E16" s="16">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="F16" s="16">
+        <v>0.78644999999999998</v>
+      </c>
+      <c r="G16" s="15">
+        <v>0.79710000000000003</v>
+      </c>
+      <c r="H16" s="15">
+        <v>0.79518</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B17" s="2">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="C17" s="22">
+        <v>0.7702</v>
+      </c>
+      <c r="D17" s="16">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="E17" s="16">
+        <v>0.7742</v>
+      </c>
+      <c r="F17" s="16">
+        <v>0.77869999999999995</v>
+      </c>
+      <c r="G17" s="15">
+        <v>0.78290000000000004</v>
+      </c>
+      <c r="H17" s="15">
+        <v>0.78449999999999998</v>
+      </c>
+      <c r="K17" s="23">
+        <v>75000</v>
+      </c>
+      <c r="L17" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="N17" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="O17" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="P17" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R17" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="S17" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="T17" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="U17" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="C18" s="22">
+        <v>0.55059999999999998</v>
+      </c>
+      <c r="D18" s="16">
+        <v>0.55659999999999998</v>
+      </c>
+      <c r="E18" s="16">
+        <v>0.55889999999999995</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="G18" s="15">
+        <v>0.56789999999999996</v>
+      </c>
+      <c r="H18" s="15">
+        <v>0.57030000000000003</v>
+      </c>
+      <c r="I18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="5"/>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="7">
+        <v>2.2677</v>
+      </c>
+      <c r="N18" s="7">
+        <v>2.0817999999999999</v>
+      </c>
+      <c r="O18" s="7">
+        <v>1.9697</v>
+      </c>
+      <c r="P18" s="7">
+        <v>1.8927</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>1.8366</v>
+      </c>
+      <c r="R18" s="7">
+        <v>1.7948999999999999</v>
+      </c>
+      <c r="S18" s="7">
+        <v>1.7652000000000001</v>
+      </c>
+      <c r="T18" s="3">
+        <v>1.7483</v>
+      </c>
+      <c r="U18" s="7">
+        <v>1.7558</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="C19" s="22">
+        <v>0.55379999999999996</v>
+      </c>
+      <c r="D19" s="16">
+        <v>0.55689999999999995</v>
+      </c>
+      <c r="E19" s="16">
+        <v>0.55620000000000003</v>
+      </c>
+      <c r="F19" s="16">
+        <v>0.55940000000000001</v>
+      </c>
+      <c r="G19" s="16">
+        <v>0.56040000000000001</v>
+      </c>
+      <c r="H19" s="15">
+        <v>0.55979999999999996</v>
+      </c>
+      <c r="I19" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="L19" s="2">
+        <f>L18+1</f>
+        <v>2</v>
+      </c>
+      <c r="M19" s="7">
+        <v>0.98909999999999998</v>
+      </c>
+      <c r="N19" s="7">
+        <v>0.97860000000000003</v>
+      </c>
+      <c r="O19" s="3">
+        <v>0.97819999999999996</v>
+      </c>
+      <c r="P19" s="7">
+        <v>0.98519999999999996</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>0.99570000000000003</v>
+      </c>
+      <c r="R19" s="7">
+        <v>1.0083</v>
+      </c>
+      <c r="S19" s="7">
+        <v>1.0230999999999999</v>
+      </c>
+      <c r="T19" s="7">
+        <v>1.0407999999999999</v>
+      </c>
+      <c r="U19" s="7">
+        <v>1.0628500000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="C20" s="22">
+        <v>0.41020000000000001</v>
+      </c>
+      <c r="D20" s="16">
+        <v>0.41889999999999999</v>
+      </c>
+      <c r="E20" s="16">
+        <v>0.42209999999999998</v>
+      </c>
+      <c r="F20" s="16">
+        <v>0.42270000000000002</v>
+      </c>
+      <c r="G20" s="15">
+        <v>0.42820000000000003</v>
+      </c>
+      <c r="H20" s="15">
+        <v>0.42949999999999999</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" ref="L20:L25" si="14">L19+1</f>
+        <v>3</v>
+      </c>
+      <c r="M20" s="7">
+        <v>0.60419999999999996</v>
+      </c>
+      <c r="N20" s="7">
+        <v>0.56310000000000004</v>
+      </c>
+      <c r="O20" s="7">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="P20" s="7">
+        <v>0.52949999999999997</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>0.52249999999999996</v>
+      </c>
+      <c r="R20" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="S20" s="7">
+        <v>0.52290000000000003</v>
+      </c>
+      <c r="T20" s="7">
+        <v>0.53420000000000001</v>
+      </c>
+      <c r="U20" s="7">
+        <v>0.56330000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B21" s="2">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="C21" s="22">
+        <v>0.30380000000000001</v>
+      </c>
+      <c r="D21" s="16">
+        <v>0.30549999999999999</v>
+      </c>
+      <c r="E21" s="16">
+        <v>0.30719999999999997</v>
+      </c>
+      <c r="F21" s="16">
+        <v>0.30840000000000001</v>
+      </c>
+      <c r="G21" s="15">
+        <v>0.31230000000000002</v>
+      </c>
+      <c r="H21" s="15">
+        <v>0.31390000000000001</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="M21" s="7">
+        <v>0.74050000000000005</v>
+      </c>
+      <c r="N21" s="7">
+        <v>0.70660000000000001</v>
+      </c>
+      <c r="O21" s="7">
+        <v>0.68520000000000003</v>
+      </c>
+      <c r="P21" s="7">
+        <v>0.67020000000000002</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>0.65890000000000004</v>
+      </c>
+      <c r="R21" s="7">
+        <v>0.64949999999999997</v>
+      </c>
+      <c r="S21" s="7">
+        <v>0.63690000000000002</v>
+      </c>
+      <c r="T21" s="7">
+        <v>0.62780000000000002</v>
+      </c>
+      <c r="U21" s="3">
+        <v>0.61480000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
+        <f>B21+1</f>
+        <v>9</v>
+      </c>
+      <c r="C22" s="16">
+        <v>0.24759999999999999</v>
+      </c>
+      <c r="D22" s="22">
+        <v>0.24729999999999999</v>
+      </c>
+      <c r="E22" s="16">
+        <v>0.25059999999999999</v>
+      </c>
+      <c r="F22" s="16">
+        <v>0.25190000000000001</v>
+      </c>
+      <c r="G22" s="15">
+        <v>0.25359999999999999</v>
+      </c>
+      <c r="H22" s="15">
+        <v>0.25389</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="M22" s="7">
+        <v>0.48570000000000002</v>
+      </c>
+      <c r="N22" s="7">
+        <v>0.46179999999999999</v>
+      </c>
+      <c r="O22" s="7">
+        <v>0.4501</v>
+      </c>
+      <c r="P22" s="7">
+        <v>0.44319999999999998</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>0.43890000000000001</v>
+      </c>
+      <c r="R22" s="7">
+        <v>0.43559999999999999</v>
+      </c>
+      <c r="S22" s="3">
+        <v>0.434</v>
+      </c>
+      <c r="T22" s="7">
+        <v>0.43619999999999998</v>
+      </c>
+      <c r="U22" s="7">
+        <v>0.44440000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="M23" s="7">
+        <v>0.54210000000000003</v>
+      </c>
+      <c r="N23" s="7">
+        <v>0.52</v>
+      </c>
+      <c r="O23" s="7">
+        <v>0.50549999999999995</v>
+      </c>
+      <c r="P23" s="7">
+        <v>0.495</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>0.48659999999999998</v>
+      </c>
+      <c r="R23" s="7">
+        <v>0.47949999999999998</v>
+      </c>
+      <c r="S23" s="7">
+        <v>0.47320000000000001</v>
+      </c>
+      <c r="T23" s="7">
+        <v>0.46650000000000003</v>
+      </c>
+      <c r="U23" s="3">
+        <v>0.46039999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="L24" s="2">
+        <f t="shared" si="14"/>
+        <v>7</v>
+      </c>
+      <c r="M24" s="7">
+        <v>0.36680000000000001</v>
+      </c>
+      <c r="N24" s="7">
+        <v>0.34279999999999999</v>
+      </c>
+      <c r="O24" s="7">
+        <v>0.3296</v>
+      </c>
+      <c r="P24" s="7">
+        <v>0.3206</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>0.31380000000000002</v>
+      </c>
+      <c r="R24" s="7">
+        <v>0.30790000000000001</v>
+      </c>
+      <c r="S24" s="7">
+        <v>0.3024</v>
+      </c>
+      <c r="T24" s="7">
+        <v>0.29670000000000002</v>
+      </c>
+      <c r="U24" s="3">
+        <v>0.28989999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="L25" s="2">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="M25" s="7">
+        <v>0.2576</v>
+      </c>
+      <c r="N25" s="7">
+        <v>0.245</v>
+      </c>
+      <c r="O25" s="7">
+        <v>0.2394</v>
+      </c>
+      <c r="P25" s="7">
+        <v>0.2326</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>0.2341</v>
+      </c>
+      <c r="R25" s="7">
+        <v>0.23180000000000001</v>
+      </c>
+      <c r="S25" s="7">
+        <v>0.2303</v>
+      </c>
+      <c r="T25" s="3">
+        <v>0.23019999999999999</v>
+      </c>
+      <c r="U25" s="7">
+        <v>0.23330000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="L26" s="2">
+        <f>L25+1</f>
+        <v>9</v>
+      </c>
+      <c r="M26" s="7">
+        <v>0.22270000000000001</v>
+      </c>
+      <c r="N26" s="7">
+        <v>0.21310000000000001</v>
+      </c>
+      <c r="O26" s="7">
+        <v>0.2082</v>
+      </c>
+      <c r="P26" s="7">
+        <v>0.2051</v>
+      </c>
+      <c r="Q26" s="7">
+        <v>0.2029</v>
+      </c>
+      <c r="R26" s="7">
+        <v>0.20030000000000001</v>
+      </c>
+      <c r="S26" s="7">
+        <v>0.19819999999999999</v>
+      </c>
+      <c r="T26" s="7">
+        <v>0.19650000000000001</v>
+      </c>
+      <c r="U26" s="3">
+        <v>0.1953</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="K29" s="23">
+        <v>25000</v>
+      </c>
+      <c r="L29" t="s">
+        <v>1</v>
+      </c>
+      <c r="M29" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="N29" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="O29" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="P29" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="Q29" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R29" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="S29" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="T29" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="U29" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="V29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="L30" s="2">
+        <v>1</v>
+      </c>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7">
+        <v>2.1429</v>
+      </c>
+      <c r="Q30" s="7">
+        <v>2.0630999999999999</v>
+      </c>
+      <c r="R30" s="7">
+        <v>1.9917</v>
+      </c>
+      <c r="S30" s="7">
+        <v>1.9281999999999999</v>
+      </c>
+      <c r="T30" s="7">
+        <v>1.8731</v>
+      </c>
+      <c r="U30" s="3">
+        <v>1.8283</v>
+      </c>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="L31" s="2">
+        <f>L30+1</f>
+        <v>2</v>
+      </c>
+      <c r="M31" s="7">
+        <v>1.0217000000000001</v>
+      </c>
+      <c r="N31" s="7">
+        <v>0.99039999999999995</v>
+      </c>
+      <c r="O31" s="7">
+        <v>0.97470000000000001</v>
+      </c>
+      <c r="P31" s="3">
+        <v>0.96919999999999995</v>
+      </c>
+      <c r="Q31" s="7">
+        <v>0.97150000000000003</v>
+      </c>
+      <c r="R31" s="7">
+        <v>0.98029999999999995</v>
+      </c>
+      <c r="S31" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T31" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U31" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="L32" s="2">
+        <f t="shared" ref="L32:L37" si="15">L31+1</f>
+        <v>3</v>
+      </c>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7">
+        <v>0.57779999999999998</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>0.56020000000000003</v>
+      </c>
+      <c r="R32" s="7">
+        <v>0.5464</v>
+      </c>
+      <c r="S32" s="7">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="T32" s="3">
+        <v>0.52929999999999999</v>
+      </c>
+      <c r="U32" s="7">
+        <v>0.52729999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="12:21" x14ac:dyDescent="0.3">
+      <c r="L33" s="2">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7">
+        <v>0.70760000000000001</v>
+      </c>
+      <c r="Q33" s="7">
+        <v>0.69440000000000002</v>
+      </c>
+      <c r="R33" s="7">
+        <v>0.68330000000000002</v>
+      </c>
+      <c r="S33" s="7">
+        <v>0.67469999999999997</v>
+      </c>
+      <c r="T33" s="3">
+        <v>0.66969999999999996</v>
+      </c>
+      <c r="U33" s="7">
+        <v>0.66759999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="12:21" x14ac:dyDescent="0.3">
+      <c r="L34" s="2">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7">
+        <v>0.45889999999999997</v>
+      </c>
+      <c r="Q34" s="7">
+        <v>0.44869999999999999</v>
+      </c>
+      <c r="R34" s="7">
+        <v>0.44140000000000001</v>
+      </c>
+      <c r="S34" s="7">
+        <v>0.437</v>
+      </c>
+      <c r="T34" s="3">
+        <v>0.43609999999999999</v>
+      </c>
+      <c r="U34" s="7">
+        <v>0.43980000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="12:21" x14ac:dyDescent="0.3">
+      <c r="L35" s="2">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7">
+        <v>0.51270000000000004</v>
+      </c>
+      <c r="Q35" s="7">
+        <v>0.50239999999999996</v>
+      </c>
+      <c r="R35" s="7">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="S35" s="7">
+        <v>0.48480000000000001</v>
+      </c>
+      <c r="T35" s="7">
+        <v>0.47820000000000001</v>
+      </c>
+      <c r="U35" s="3">
+        <v>0.47420000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="12:21" x14ac:dyDescent="0.3">
+      <c r="L36" s="2">
+        <f t="shared" si="15"/>
+        <v>7</v>
+      </c>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7">
+        <v>0.3387</v>
+      </c>
+      <c r="Q36" s="7">
+        <v>0.3281</v>
+      </c>
+      <c r="R36" s="7">
+        <v>0.31919999999999998</v>
+      </c>
+      <c r="S36" s="7">
+        <v>0.31169999999999998</v>
+      </c>
+      <c r="T36" s="7">
+        <v>0.3054</v>
+      </c>
+      <c r="U36" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="37" spans="12:21" x14ac:dyDescent="0.3">
+      <c r="L37" s="2">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7">
+        <v>0.24909999999999999</v>
+      </c>
+      <c r="Q37" s="7">
+        <v>0.245</v>
+      </c>
+      <c r="R37" s="7">
+        <v>0.24260000000000001</v>
+      </c>
+      <c r="S37" s="3">
+        <v>0.24210000000000001</v>
+      </c>
+      <c r="T37" s="7">
+        <v>0.24360000000000001</v>
+      </c>
+      <c r="U37" s="7">
+        <v>0.24740000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="12:21" x14ac:dyDescent="0.3">
+      <c r="L38" s="2">
+        <f>L37+1</f>
+        <v>9</v>
+      </c>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7">
+        <v>0.21540000000000001</v>
+      </c>
+      <c r="Q38" s="7">
+        <v>0.2117</v>
+      </c>
+      <c r="R38" s="7">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="S38" s="7">
+        <v>0.20730000000000001</v>
+      </c>
+      <c r="T38" s="3">
+        <v>0.20669999999999999</v>
+      </c>
+      <c r="U38" s="7">
+        <v>0.2074</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>